<commit_message>
GUI + API test update 1
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -11,7 +11,11 @@
     <sheet name="login" sheetId="2" r:id="rId2"/>
     <sheet name="Configuration details" sheetId="3" r:id="rId3"/>
     <sheet name="createQuestionManually" sheetId="4" r:id="rId4"/>
+    <sheet name="editQuestion" sheetId="5" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">createQuestionManually!$A$14:$B$24</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -21,8 +25,32 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="B3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Append/Change
+It will define the que will be edit or change thoroughly</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="71">
   <si>
     <t>id</t>
   </si>
@@ -174,14 +202,106 @@
     <t>Objective</t>
   </si>
   <si>
-    <t>First question by automation.</t>
+    <t>CreateQuestion Manually API</t>
+  </si>
+  <si>
+    <t>http://192.168.91.48/api/v1/AssessmentQuestion</t>
+  </si>
+  <si>
+    <t>updatedQuestion</t>
+  </si>
+  <si>
+    <t>Hey I'm updated text in the question</t>
+  </si>
+  <si>
+    <t>editType</t>
+  </si>
+  <si>
+    <t>Append</t>
+  </si>
+  <si>
+    <t>http://192.168.91.48/api/v1/AssessmentQuestion/AssessmentQuestionExist</t>
+  </si>
+  <si>
+    <t>API request1</t>
+  </si>
+  <si>
+    <t>Method1</t>
+  </si>
+  <si>
+    <t>Parameter json1</t>
+  </si>
+  <si>
+    <t>Expected response code2</t>
+  </si>
+  <si>
+    <t>Expected response body</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>API request2</t>
+  </si>
+  <si>
+    <t>Method2</t>
+  </si>
+  <si>
+    <t>Parameter json2</t>
+  </si>
+  <si>
+    <t>header2</t>
+  </si>
+  <si>
+    <t>Expected response code1</t>
+  </si>
+  <si>
+    <t>Quee 11</t>
+  </si>
+  <si>
+    <t>{
+  "QuestionText": "Test Que 51"
+}</t>
+  </si>
+  <si>
+    <t>[
+  {
+    "section": "objective",
+    "subjectiveAnswerLimit": 1,
+    "questionText": "Test Que 51",
+    "questionStyle": "orderbydesending",
+    "OptionType": "SingleSelection",
+    "randomizedQuestion": false,
+    "marks": 1,
+    "status": true,
+    "IsMemoQuestion": false,
+    "options": 2,
+    "metadata": "test4",
+    "difficultylevel": "Simple",
+    "contentType": "Objective",
+    "aPIAssessmentOptions": [
+      {
+        "optionText": "aaa1",
+        "isCorrectAnswer": true,
+        "contentPath": "",
+        "contentType": ""
+      },
+      {
+        "optionText": "bbbb",
+        "isCorrectAnswer": false,
+        "contentPath": "",
+        "contentType": ""
+      }
+    ]
+  }
+]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,6 +325,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF505050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -227,7 +365,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -238,6 +376,11 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -522,7 +665,7 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,7 +778,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,8 +852,8 @@
       <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="4">
-        <v>200</v>
+      <c r="B9" s="4" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -770,16 +913,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -795,7 +938,7 @@
         <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -884,10 +1027,139 @@
       </c>
       <c r="B13" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>